<commit_message>
refactor and new experiments
</commit_message>
<xml_diff>
--- a/experiments_results/Indice_Experimentos.xlsx
+++ b/experiments_results/Indice_Experimentos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\apa\elastic-smart-contracts\experiments_results\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80AC6542-8BBA-4D15-A266-4E3E8AD1FF02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9C94EEB-1791-43F4-8416-E891E4122015}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{C605E24C-3C93-43B7-80BE-30E8D3278DB9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C605E24C-3C93-43B7-80BE-30E8D3278DB9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="60">
   <si>
     <t>ID</t>
   </si>
@@ -109,9 +109,6 @@
     <t>Frecuencia recoleccion</t>
   </si>
   <si>
-    <t>2.5</t>
-  </si>
-  <si>
     <t>Experimento14</t>
   </si>
   <si>
@@ -119,9 +116,6 @@
   </si>
   <si>
     <t>ColdStart=True</t>
-  </si>
-  <si>
-    <t>3.2</t>
   </si>
   <si>
     <t>ColdStart=True
@@ -158,9 +152,6 @@
     <t>Experimento12</t>
   </si>
   <si>
-    <t>Experimento12 with a sleep(60) between esc</t>
-  </si>
-  <si>
     <t>Experimento21 with a final sleep(1200)</t>
   </si>
   <si>
@@ -204,6 +195,27 @@
   </si>
   <si>
     <t>Experimento30</t>
+  </si>
+  <si>
+    <t>Elasticity with average of 5 last times</t>
+  </si>
+  <si>
+    <t>Experimento29 with sleep(600) between ESC</t>
+  </si>
+  <si>
+    <t>Experimento29 with sleep(300) between ESC</t>
+  </si>
+  <si>
+    <t>Experimento32</t>
+  </si>
+  <si>
+    <t>Experimento33</t>
+  </si>
+  <si>
+    <t>Experimento29 with sleep(1200) between ESC</t>
+  </si>
+  <si>
+    <t>Experimento12 with a sleep(60) between ESC</t>
   </si>
 </sst>
 </file>
@@ -268,7 +280,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -564,28 +576,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06659444-A726-49AD-A5E7-7ED3AC17F9D5}">
-  <dimension ref="A1:L83"/>
+  <dimension ref="A1:L93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B62" workbookViewId="0">
-      <selection activeCell="L84" sqref="L84"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="41.109375" customWidth="1"/>
-    <col min="3" max="3" width="13.44140625" customWidth="1"/>
-    <col min="4" max="4" width="20.5546875" customWidth="1"/>
-    <col min="5" max="5" width="15.6640625" customWidth="1"/>
-    <col min="6" max="6" width="34.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.88671875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.88671875" customWidth="1"/>
-    <col min="10" max="10" width="27.6640625" customWidth="1"/>
+    <col min="2" max="2" width="41.5703125" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" customWidth="1"/>
+    <col min="4" max="4" width="20.5703125" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" customWidth="1"/>
+    <col min="6" max="6" width="34.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.85546875" customWidth="1"/>
+    <col min="10" max="10" width="27.7109375" customWidth="1"/>
     <col min="11" max="11" width="16" customWidth="1"/>
-    <col min="12" max="12" width="14.6640625" customWidth="1"/>
+    <col min="12" max="12" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -623,7 +635,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -658,7 +670,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -693,7 +705,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -728,7 +740,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -763,7 +775,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -798,7 +810,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -833,7 +845,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -868,7 +880,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -903,7 +915,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -938,7 +950,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -973,7 +985,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1008,7 +1020,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1043,7 +1055,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1078,7 +1090,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1113,7 +1125,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1148,7 +1160,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1183,7 +1195,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1218,7 +1230,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1253,7 +1265,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1288,12 +1300,12 @@
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C21">
         <v>1</v>
@@ -1323,12 +1335,12 @@
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C22">
         <v>4</v>
@@ -1358,7 +1370,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1393,12 +1405,12 @@
         <v>11</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C24">
         <v>1</v>
@@ -1428,7 +1440,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1463,7 +1475,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1498,12 +1510,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C27">
         <v>4</v>
@@ -1533,12 +1545,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C28">
         <v>4</v>
@@ -1568,12 +1580,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C29">
         <v>16</v>
@@ -1603,12 +1615,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>30</v>
       </c>
       <c r="B30" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C30">
         <v>16</v>
@@ -1638,12 +1650,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>31</v>
       </c>
       <c r="B31" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C31">
         <v>16</v>
@@ -1673,12 +1685,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>32</v>
       </c>
       <c r="B32" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C32">
         <v>16</v>
@@ -1708,12 +1720,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>33</v>
       </c>
       <c r="B33" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C33">
         <v>16</v>
@@ -1743,12 +1755,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>34</v>
       </c>
       <c r="B34" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C34">
         <v>1</v>
@@ -1778,12 +1790,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>35</v>
       </c>
       <c r="B35" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C35">
         <v>1</v>
@@ -1813,12 +1825,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>36</v>
       </c>
       <c r="B36" t="s">
-        <v>40</v>
+        <v>59</v>
       </c>
       <c r="C36">
         <v>4</v>
@@ -1848,12 +1860,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>37</v>
       </c>
       <c r="B37" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C37">
         <v>16</v>
@@ -1883,12 +1895,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>38</v>
       </c>
       <c r="B38" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C38">
         <v>4</v>
@@ -1918,12 +1930,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>40</v>
       </c>
       <c r="B39" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C39">
         <v>1</v>
@@ -1937,8 +1949,8 @@
       <c r="F39">
         <v>1</v>
       </c>
-      <c r="G39" t="s">
-        <v>24</v>
+      <c r="G39">
+        <v>2.5</v>
       </c>
       <c r="H39">
         <v>3</v>
@@ -1953,12 +1965,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>41</v>
       </c>
       <c r="B40" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C40">
         <v>2</v>
@@ -1972,8 +1984,8 @@
       <c r="F40">
         <v>2</v>
       </c>
-      <c r="G40" t="s">
-        <v>24</v>
+      <c r="G40">
+        <v>2.5</v>
       </c>
       <c r="H40">
         <v>3</v>
@@ -1988,12 +2000,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>42</v>
       </c>
       <c r="B41" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C41">
         <v>4</v>
@@ -2007,8 +2019,8 @@
       <c r="F41">
         <v>4</v>
       </c>
-      <c r="G41" t="s">
-        <v>24</v>
+      <c r="G41">
+        <v>2.5</v>
       </c>
       <c r="H41">
         <v>3</v>
@@ -2023,12 +2035,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>43</v>
       </c>
       <c r="B42" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C42">
         <v>8</v>
@@ -2042,8 +2054,8 @@
       <c r="F42">
         <v>8</v>
       </c>
-      <c r="G42" t="s">
-        <v>24</v>
+      <c r="G42">
+        <v>2.5</v>
       </c>
       <c r="H42">
         <v>3</v>
@@ -2058,12 +2070,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>44</v>
       </c>
       <c r="B43" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C43">
         <v>16</v>
@@ -2077,8 +2089,8 @@
       <c r="F43">
         <v>16</v>
       </c>
-      <c r="G43" t="s">
-        <v>24</v>
+      <c r="G43">
+        <v>2.5</v>
       </c>
       <c r="H43">
         <v>3</v>
@@ -2093,12 +2105,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>45</v>
       </c>
       <c r="B44" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C44">
         <v>16</v>
@@ -2112,8 +2124,8 @@
       <c r="F44">
         <v>16</v>
       </c>
-      <c r="G44" t="s">
-        <v>24</v>
+      <c r="G44">
+        <v>2.5</v>
       </c>
       <c r="H44">
         <v>3</v>
@@ -2128,12 +2140,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>46</v>
       </c>
       <c r="B45" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C45">
         <v>1</v>
@@ -2147,8 +2159,8 @@
       <c r="F45">
         <v>1</v>
       </c>
-      <c r="G45" t="s">
-        <v>24</v>
+      <c r="G45">
+        <v>2.5</v>
       </c>
       <c r="H45">
         <v>3</v>
@@ -2163,12 +2175,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>47</v>
       </c>
       <c r="B46" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C46">
         <v>8</v>
@@ -2182,8 +2194,8 @@
       <c r="F46">
         <v>8</v>
       </c>
-      <c r="G46" t="s">
-        <v>24</v>
+      <c r="G46">
+        <v>2.5</v>
       </c>
       <c r="H46">
         <v>3</v>
@@ -2198,12 +2210,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>51</v>
       </c>
       <c r="B47" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C47">
         <v>2</v>
@@ -2217,8 +2229,8 @@
       <c r="F47">
         <v>2</v>
       </c>
-      <c r="G47" t="s">
-        <v>24</v>
+      <c r="G47">
+        <v>2.5</v>
       </c>
       <c r="H47">
         <v>3</v>
@@ -2227,7 +2239,7 @@
         <v>17</v>
       </c>
       <c r="J47" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K47">
         <v>15</v>
@@ -2236,12 +2248,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>52</v>
       </c>
       <c r="B48" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C48">
         <v>4</v>
@@ -2255,8 +2267,8 @@
       <c r="F48">
         <v>4</v>
       </c>
-      <c r="G48" t="s">
-        <v>24</v>
+      <c r="G48">
+        <v>2.5</v>
       </c>
       <c r="H48">
         <v>3</v>
@@ -2265,7 +2277,7 @@
         <v>17</v>
       </c>
       <c r="J48" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K48">
         <v>15</v>
@@ -2274,12 +2286,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>53</v>
       </c>
       <c r="B49" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C49">
         <v>8</v>
@@ -2293,8 +2305,8 @@
       <c r="F49">
         <v>8</v>
       </c>
-      <c r="G49" t="s">
-        <v>24</v>
+      <c r="G49">
+        <v>2.5</v>
       </c>
       <c r="H49">
         <v>3</v>
@@ -2303,7 +2315,7 @@
         <v>17</v>
       </c>
       <c r="J49" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K49">
         <v>15</v>
@@ -2312,12 +2324,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>54</v>
       </c>
       <c r="B50" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C50">
         <v>16</v>
@@ -2331,8 +2343,8 @@
       <c r="F50">
         <v>16</v>
       </c>
-      <c r="G50" t="s">
-        <v>24</v>
+      <c r="G50">
+        <v>2.5</v>
       </c>
       <c r="H50">
         <v>3</v>
@@ -2341,7 +2353,7 @@
         <v>17</v>
       </c>
       <c r="J50" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K50">
         <v>15</v>
@@ -2350,12 +2362,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>55</v>
       </c>
       <c r="B51" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C51">
         <v>1</v>
@@ -2372,14 +2384,14 @@
       <c r="G51">
         <v>3</v>
       </c>
-      <c r="H51" t="s">
-        <v>28</v>
+      <c r="H51">
+        <v>3.2</v>
       </c>
       <c r="I51" t="s">
         <v>18</v>
       </c>
       <c r="J51" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K51">
         <v>15</v>
@@ -2388,12 +2400,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>56</v>
       </c>
       <c r="B52" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C52">
         <v>2</v>
@@ -2410,14 +2422,14 @@
       <c r="G52">
         <v>3</v>
       </c>
-      <c r="H52" t="s">
-        <v>28</v>
+      <c r="H52">
+        <v>3.2</v>
       </c>
       <c r="I52" t="s">
         <v>18</v>
       </c>
       <c r="J52" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K52">
         <v>15</v>
@@ -2426,12 +2438,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>57</v>
       </c>
       <c r="B53" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C53">
         <v>4</v>
@@ -2448,14 +2460,14 @@
       <c r="G53">
         <v>3</v>
       </c>
-      <c r="H53" t="s">
-        <v>28</v>
+      <c r="H53">
+        <v>3.2</v>
       </c>
       <c r="I53" t="s">
         <v>18</v>
       </c>
       <c r="J53" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K53">
         <v>15</v>
@@ -2464,12 +2476,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>58</v>
       </c>
       <c r="B54" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C54">
         <v>8</v>
@@ -2486,14 +2498,14 @@
       <c r="G54">
         <v>3</v>
       </c>
-      <c r="H54" t="s">
-        <v>28</v>
+      <c r="H54">
+        <v>3.2</v>
       </c>
       <c r="I54" t="s">
         <v>18</v>
       </c>
       <c r="J54" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K54">
         <v>15</v>
@@ -2502,12 +2514,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>59</v>
       </c>
       <c r="B55" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C55">
         <v>16</v>
@@ -2524,14 +2536,14 @@
       <c r="G55">
         <v>3</v>
       </c>
-      <c r="H55" t="s">
-        <v>28</v>
+      <c r="H55">
+        <v>3.2</v>
       </c>
       <c r="I55" t="s">
         <v>18</v>
       </c>
       <c r="J55" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K55">
         <v>15</v>
@@ -2540,12 +2552,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>62</v>
       </c>
       <c r="B56" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C56">
         <v>2</v>
@@ -2562,14 +2574,14 @@
       <c r="G56">
         <v>3</v>
       </c>
-      <c r="H56" t="s">
-        <v>28</v>
+      <c r="H56">
+        <v>3.2</v>
       </c>
       <c r="I56" t="s">
         <v>18</v>
       </c>
       <c r="J56" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K56">
         <v>15</v>
@@ -2578,12 +2590,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>63</v>
       </c>
       <c r="B57" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C57">
         <v>4</v>
@@ -2600,14 +2612,14 @@
       <c r="G57">
         <v>3</v>
       </c>
-      <c r="H57" t="s">
-        <v>28</v>
+      <c r="H57">
+        <v>3.2</v>
       </c>
       <c r="I57" t="s">
         <v>18</v>
       </c>
       <c r="J57" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K57">
         <v>15</v>
@@ -2616,12 +2628,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>64</v>
       </c>
       <c r="B58" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C58">
         <v>8</v>
@@ -2638,14 +2650,14 @@
       <c r="G58">
         <v>3</v>
       </c>
-      <c r="H58" t="s">
-        <v>28</v>
+      <c r="H58">
+        <v>3.2</v>
       </c>
       <c r="I58" t="s">
         <v>18</v>
       </c>
       <c r="J58" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K58">
         <v>15</v>
@@ -2654,12 +2666,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>65</v>
       </c>
       <c r="B59" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C59">
         <v>16</v>
@@ -2676,14 +2688,14 @@
       <c r="G59">
         <v>3</v>
       </c>
-      <c r="H59" t="s">
-        <v>28</v>
+      <c r="H59">
+        <v>3.2</v>
       </c>
       <c r="I59" t="s">
         <v>18</v>
       </c>
       <c r="J59" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K59">
         <v>15</v>
@@ -2692,12 +2704,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="60" spans="1:12" ht="37.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:12" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>66</v>
       </c>
       <c r="B60" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C60">
         <v>2</v>
@@ -2714,14 +2726,14 @@
       <c r="G60">
         <v>3</v>
       </c>
-      <c r="H60" t="s">
-        <v>28</v>
+      <c r="H60">
+        <v>3.2</v>
       </c>
       <c r="I60" t="s">
         <v>18</v>
       </c>
       <c r="J60" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="K60">
         <v>15</v>
@@ -2730,12 +2742,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="61" spans="1:12" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:12" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>67</v>
       </c>
       <c r="B61" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C61">
         <v>4</v>
@@ -2752,14 +2764,14 @@
       <c r="G61">
         <v>3</v>
       </c>
-      <c r="H61" t="s">
-        <v>28</v>
+      <c r="H61">
+        <v>3.2</v>
       </c>
       <c r="I61" t="s">
         <v>18</v>
       </c>
       <c r="J61" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="K61">
         <v>15</v>
@@ -2768,12 +2780,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="62" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>68</v>
       </c>
       <c r="B62" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C62">
         <v>8</v>
@@ -2790,14 +2802,14 @@
       <c r="G62">
         <v>3</v>
       </c>
-      <c r="H62" t="s">
-        <v>28</v>
+      <c r="H62">
+        <v>3.2</v>
       </c>
       <c r="I62" t="s">
         <v>18</v>
       </c>
       <c r="J62" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="K62">
         <v>15</v>
@@ -2806,12 +2818,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>69</v>
       </c>
       <c r="B63" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C63">
         <v>4</v>
@@ -2828,14 +2840,14 @@
       <c r="G63">
         <v>3</v>
       </c>
-      <c r="H63" t="s">
-        <v>28</v>
+      <c r="H63">
+        <v>3.2</v>
       </c>
       <c r="I63" t="s">
         <v>18</v>
       </c>
       <c r="J63" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K63">
         <v>15</v>
@@ -2844,12 +2856,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>70</v>
       </c>
       <c r="B64" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C64">
         <v>2</v>
@@ -2866,14 +2878,14 @@
       <c r="G64">
         <v>3</v>
       </c>
-      <c r="H64" t="s">
-        <v>28</v>
+      <c r="H64">
+        <v>3.2</v>
       </c>
       <c r="I64" t="s">
         <v>17</v>
       </c>
       <c r="J64" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K64">
         <v>15</v>
@@ -2882,12 +2894,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>71</v>
       </c>
       <c r="B65" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C65">
         <v>4</v>
@@ -2904,14 +2916,14 @@
       <c r="G65">
         <v>3</v>
       </c>
-      <c r="H65" t="s">
-        <v>28</v>
+      <c r="H65">
+        <v>3.2</v>
       </c>
       <c r="I65" t="s">
         <v>17</v>
       </c>
       <c r="J65" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K65">
         <v>15</v>
@@ -2920,12 +2932,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>72</v>
       </c>
       <c r="B66" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C66">
         <v>8</v>
@@ -2942,14 +2954,14 @@
       <c r="G66">
         <v>3</v>
       </c>
-      <c r="H66" t="s">
-        <v>28</v>
+      <c r="H66">
+        <v>3.2</v>
       </c>
       <c r="I66" t="s">
         <v>17</v>
       </c>
       <c r="J66" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K66">
         <v>15</v>
@@ -2958,12 +2970,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>73</v>
       </c>
       <c r="B67" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C67">
         <v>16</v>
@@ -2980,14 +2992,14 @@
       <c r="G67">
         <v>3</v>
       </c>
-      <c r="H67" t="s">
-        <v>28</v>
+      <c r="H67">
+        <v>3.2</v>
       </c>
       <c r="I67" t="s">
         <v>17</v>
       </c>
       <c r="J67" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K67">
         <v>15</v>
@@ -2996,12 +3008,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>74</v>
       </c>
       <c r="B68" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C68">
         <v>16</v>
@@ -3018,8 +3030,8 @@
       <c r="G68">
         <v>3</v>
       </c>
-      <c r="H68" t="s">
-        <v>28</v>
+      <c r="H68">
+        <v>3.2</v>
       </c>
       <c r="I68" t="s">
         <v>17</v>
@@ -3032,12 +3044,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>76</v>
       </c>
       <c r="B69" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C69">
         <v>16</v>
@@ -3054,14 +3066,14 @@
       <c r="G69">
         <v>3</v>
       </c>
-      <c r="H69" t="s">
-        <v>28</v>
+      <c r="H69">
+        <v>3.2</v>
       </c>
       <c r="I69" t="s">
         <v>17</v>
       </c>
       <c r="J69" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K69">
         <v>15</v>
@@ -3070,12 +3082,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>77</v>
       </c>
       <c r="B70" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C70">
         <v>16</v>
@@ -3092,8 +3104,8 @@
       <c r="G70">
         <v>3</v>
       </c>
-      <c r="H70" t="s">
-        <v>28</v>
+      <c r="H70">
+        <v>3.2</v>
       </c>
       <c r="I70" t="s">
         <v>17</v>
@@ -3106,12 +3118,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>78</v>
       </c>
       <c r="B71" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C71">
         <v>4</v>
@@ -3128,8 +3140,8 @@
       <c r="G71">
         <v>3</v>
       </c>
-      <c r="H71" t="s">
-        <v>28</v>
+      <c r="H71">
+        <v>3.2</v>
       </c>
       <c r="I71" t="s">
         <v>17</v>
@@ -3142,12 +3154,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>80</v>
       </c>
       <c r="B72" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C72">
         <v>2</v>
@@ -3171,7 +3183,7 @@
         <v>17</v>
       </c>
       <c r="J72" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K72">
         <v>5</v>
@@ -3180,12 +3192,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>81</v>
       </c>
       <c r="B73" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C73">
         <v>2</v>
@@ -3209,7 +3221,7 @@
         <v>17</v>
       </c>
       <c r="J73" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K73">
         <v>15</v>
@@ -3218,12 +3230,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>82</v>
       </c>
       <c r="B74" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C74">
         <v>2</v>
@@ -3247,7 +3259,7 @@
         <v>18</v>
       </c>
       <c r="J74" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K74">
         <v>15</v>
@@ -3256,12 +3268,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>83</v>
       </c>
       <c r="B75" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C75">
         <v>2</v>
@@ -3285,7 +3297,7 @@
         <v>18</v>
       </c>
       <c r="J75" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K75">
         <v>5</v>
@@ -3294,12 +3306,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>84</v>
       </c>
       <c r="B76" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C76">
         <v>2</v>
@@ -3330,12 +3342,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>85</v>
       </c>
       <c r="B77" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C77">
         <v>2</v>
@@ -3366,12 +3378,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>86</v>
       </c>
       <c r="B78" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C78">
         <v>2</v>
@@ -3402,12 +3414,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>87</v>
       </c>
       <c r="B79" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C79">
         <v>2</v>
@@ -3438,12 +3450,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>88</v>
       </c>
       <c r="B80" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C80">
         <v>2</v>
@@ -3467,7 +3479,7 @@
         <v>17</v>
       </c>
       <c r="J80" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="K80">
         <v>15</v>
@@ -3476,12 +3488,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>89</v>
       </c>
       <c r="B81" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C81">
         <v>2</v>
@@ -3505,7 +3517,7 @@
         <v>17</v>
       </c>
       <c r="J81" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="K81">
         <v>15</v>
@@ -3514,12 +3526,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>90</v>
       </c>
       <c r="B82" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C82">
         <v>2</v>
@@ -3543,7 +3555,7 @@
         <v>17</v>
       </c>
       <c r="J82" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="K82">
         <v>15</v>
@@ -3552,12 +3564,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>91</v>
       </c>
       <c r="B83" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C83">
         <v>2</v>
@@ -3581,13 +3593,393 @@
         <v>17</v>
       </c>
       <c r="J83" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="K83">
         <v>5</v>
       </c>
       <c r="L83">
         <v>5</v>
+      </c>
+    </row>
+    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <v>92</v>
+      </c>
+      <c r="B84" t="s">
+        <v>50</v>
+      </c>
+      <c r="C84">
+        <v>2</v>
+      </c>
+      <c r="D84">
+        <v>1200</v>
+      </c>
+      <c r="E84">
+        <v>300</v>
+      </c>
+      <c r="F84">
+        <v>1</v>
+      </c>
+      <c r="G84">
+        <v>3</v>
+      </c>
+      <c r="H84">
+        <v>3.2</v>
+      </c>
+      <c r="I84" t="s">
+        <v>17</v>
+      </c>
+      <c r="J84" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="K84">
+        <v>5</v>
+      </c>
+      <c r="L84">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="85" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <v>93</v>
+      </c>
+      <c r="B85" t="s">
+        <v>50</v>
+      </c>
+      <c r="C85">
+        <v>2</v>
+      </c>
+      <c r="D85">
+        <v>1200</v>
+      </c>
+      <c r="E85">
+        <v>300</v>
+      </c>
+      <c r="F85">
+        <v>1</v>
+      </c>
+      <c r="G85">
+        <v>3</v>
+      </c>
+      <c r="H85">
+        <v>3.2</v>
+      </c>
+      <c r="I85" t="s">
+        <v>17</v>
+      </c>
+      <c r="J85" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="K85">
+        <v>30</v>
+      </c>
+      <c r="L85">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="86" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <v>94</v>
+      </c>
+      <c r="B86" t="s">
+        <v>52</v>
+      </c>
+      <c r="C86">
+        <v>2</v>
+      </c>
+      <c r="D86">
+        <v>3600</v>
+      </c>
+      <c r="E86">
+        <v>900</v>
+      </c>
+      <c r="F86">
+        <v>1</v>
+      </c>
+      <c r="G86">
+        <v>3</v>
+      </c>
+      <c r="H86">
+        <v>3.2</v>
+      </c>
+      <c r="I86" t="s">
+        <v>17</v>
+      </c>
+      <c r="J86" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="K86">
+        <v>30</v>
+      </c>
+      <c r="L86">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="87" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <v>95</v>
+      </c>
+      <c r="B87" t="s">
+        <v>54</v>
+      </c>
+      <c r="C87">
+        <v>2</v>
+      </c>
+      <c r="D87">
+        <v>2400</v>
+      </c>
+      <c r="E87">
+        <v>600</v>
+      </c>
+      <c r="F87">
+        <v>1</v>
+      </c>
+      <c r="G87">
+        <v>3</v>
+      </c>
+      <c r="H87">
+        <v>3.2</v>
+      </c>
+      <c r="I87" t="s">
+        <v>17</v>
+      </c>
+      <c r="J87" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="K87">
+        <v>30</v>
+      </c>
+      <c r="L87">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="88" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A88">
+        <v>96</v>
+      </c>
+      <c r="B88" t="s">
+        <v>55</v>
+      </c>
+      <c r="C88">
+        <v>2</v>
+      </c>
+      <c r="D88">
+        <v>1800</v>
+      </c>
+      <c r="E88">
+        <v>300</v>
+      </c>
+      <c r="F88">
+        <v>1</v>
+      </c>
+      <c r="G88">
+        <v>3</v>
+      </c>
+      <c r="H88">
+        <v>3.2</v>
+      </c>
+      <c r="I88" t="s">
+        <v>17</v>
+      </c>
+      <c r="J88" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="K88">
+        <v>30</v>
+      </c>
+      <c r="L88">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="89" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A89">
+        <v>97</v>
+      </c>
+      <c r="B89" t="s">
+        <v>56</v>
+      </c>
+      <c r="C89">
+        <v>1</v>
+      </c>
+      <c r="D89">
+        <v>900</v>
+      </c>
+      <c r="E89">
+        <v>0</v>
+      </c>
+      <c r="F89">
+        <v>1</v>
+      </c>
+      <c r="G89">
+        <v>3</v>
+      </c>
+      <c r="H89">
+        <v>3.2</v>
+      </c>
+      <c r="I89" t="s">
+        <v>17</v>
+      </c>
+      <c r="J89" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="K89">
+        <v>30</v>
+      </c>
+      <c r="L89">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="90" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A90">
+        <v>98</v>
+      </c>
+      <c r="B90" t="s">
+        <v>57</v>
+      </c>
+      <c r="C90">
+        <v>3</v>
+      </c>
+      <c r="D90">
+        <v>2400</v>
+      </c>
+      <c r="E90">
+        <v>300</v>
+      </c>
+      <c r="F90">
+        <v>1</v>
+      </c>
+      <c r="G90">
+        <v>3</v>
+      </c>
+      <c r="H90">
+        <v>3.2</v>
+      </c>
+      <c r="I90" t="s">
+        <v>17</v>
+      </c>
+      <c r="J90" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="K90">
+        <v>30</v>
+      </c>
+      <c r="L90">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="91" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A91">
+        <v>99</v>
+      </c>
+      <c r="B91" t="s">
+        <v>57</v>
+      </c>
+      <c r="C91">
+        <v>3</v>
+      </c>
+      <c r="D91">
+        <v>2400</v>
+      </c>
+      <c r="E91">
+        <v>300</v>
+      </c>
+      <c r="F91">
+        <v>1</v>
+      </c>
+      <c r="G91">
+        <v>3</v>
+      </c>
+      <c r="H91">
+        <v>3.2</v>
+      </c>
+      <c r="I91" t="s">
+        <v>17</v>
+      </c>
+      <c r="J91" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="K91">
+        <v>30</v>
+      </c>
+      <c r="L91">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="92" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A92">
+        <v>100</v>
+      </c>
+      <c r="B92" t="s">
+        <v>55</v>
+      </c>
+      <c r="C92">
+        <v>2</v>
+      </c>
+      <c r="D92">
+        <v>1800</v>
+      </c>
+      <c r="E92">
+        <v>300</v>
+      </c>
+      <c r="F92">
+        <v>1</v>
+      </c>
+      <c r="G92">
+        <v>3</v>
+      </c>
+      <c r="H92">
+        <v>3.2</v>
+      </c>
+      <c r="I92" t="s">
+        <v>17</v>
+      </c>
+      <c r="J92" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="K92">
+        <v>30</v>
+      </c>
+      <c r="L92">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="93" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A93">
+        <v>102</v>
+      </c>
+      <c r="B93" t="s">
+        <v>58</v>
+      </c>
+      <c r="C93">
+        <v>2</v>
+      </c>
+      <c r="D93">
+        <v>1500</v>
+      </c>
+      <c r="E93">
+        <v>300</v>
+      </c>
+      <c r="F93">
+        <v>1</v>
+      </c>
+      <c r="G93">
+        <v>3</v>
+      </c>
+      <c r="H93">
+        <v>3.2</v>
+      </c>
+      <c r="I93" t="s">
+        <v>17</v>
+      </c>
+      <c r="J93" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="K93">
+        <v>30</v>
+      </c>
+      <c r="L93">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>